<commit_message>
screenshots of database and scraped data
</commit_message>
<xml_diff>
--- a/values.xlsx
+++ b/values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trent\Downloads\UTK_School\UTKSeniorYear\UTKFall2021\CS445\fantasyfootball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD3414A-B80F-404D-93B1-2DD034A77A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39898909-2CA2-45D8-AA94-B08777BF4072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I901"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A814" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+      <selection activeCell="L430" sqref="L430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>